<commit_message>
Test, add xmlids to pacscl TEI
</commit_message>
<xml_diff>
--- a/openn/tests/data/diaries/haverford/MC_968_11_4_v03/openn_metadata.xlsx
+++ b/openn/tests/data/diaries/haverford/MC_968_11_4_v03/openn_metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="3752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="3754">
   <si>
     <t>1r</t>
   </si>
@@ -11323,6 +11323,12 @@
   </si>
   <si>
     <t>Haverford College</t>
+  </si>
+  <si>
+    <t>It's a duck</t>
+  </si>
+  <si>
+    <t>Beginning of a section</t>
   </si>
 </sst>
 </file>
@@ -11874,7 +11880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -13100,9 +13106,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13313,8 +13319,12 @@
       <c r="D10" s="19" t="s">
         <v>3719</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>2620</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>3752</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="15"/>
       <c r="I10" s="2"/>
@@ -13332,8 +13342,12 @@
       <c r="D11" s="19" t="s">
         <v>3720</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="2" t="s">
+        <v>2617</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>3753</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="15"/>
       <c r="I11" s="2"/>

</xml_diff>